<commit_message>
Correct total token count in % calculations, added additional measures for negative count with unemployment included, as well as separate positive and negative %
</commit_message>
<xml_diff>
--- a/Descriptive stats file.xlsx
+++ b/Descriptive stats file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Honours-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43BF3B6-2B40-4D1D-8129-5ED704DB61DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0456A4AC-3EE4-4263-81AC-424F9785F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Dates</t>
   </si>
@@ -105,12 +105,18 @@
   <si>
     <t>Confidence Level(95.0%)</t>
   </si>
+  <si>
+    <t>Glen Stevens</t>
+  </si>
+  <si>
+    <t>Phillip Lowe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +138,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -222,6 +236,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4546,13 +4561,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AA22" sqref="AA22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4578,6 +4593,12 @@
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
@@ -4606,6 +4627,12 @@
         <f>G2*-1</f>
         <v>-1.5995260663507111E-2</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
@@ -4634,6 +4661,12 @@
         <f t="shared" ref="H3:H66" si="1">G3*-1</f>
         <v>-1.7137096774193551E-2</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="AE3" t="s">
         <v>8</v>
       </c>
@@ -4665,6 +4698,12 @@
         <f t="shared" si="1"/>
         <v>-2.4421593830334189E-2</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
@@ -4693,6 +4732,12 @@
         <f t="shared" si="1"/>
         <v>-1.434809731752963E-2</v>
       </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
@@ -4721,6 +4766,12 @@
         <f t="shared" si="1"/>
         <v>-2.602739726027397E-2</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -4749,6 +4800,12 @@
         <f t="shared" si="1"/>
         <v>-6.7618332081142004E-3</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
@@ -4777,6 +4834,12 @@
         <f t="shared" si="1"/>
         <v>-1.328021248339973E-2</v>
       </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
@@ -4805,6 +4868,12 @@
         <f t="shared" si="1"/>
         <v>2.0449897750511249E-3</v>
       </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
@@ -4833,6 +4902,12 @@
         <f t="shared" si="1"/>
         <v>-3.3314825097168241E-3</v>
       </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
@@ -4861,6 +4936,12 @@
         <f t="shared" si="1"/>
         <v>-1.819284414796847E-2</v>
       </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
@@ -4889,6 +4970,12 @@
         <f t="shared" si="1"/>
         <v>-1.5889830508474579E-2</v>
       </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
@@ -4917,6 +5004,12 @@
         <f t="shared" si="1"/>
         <v>-1.5033072760072159E-2</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
@@ -4945,6 +5038,12 @@
         <f t="shared" si="1"/>
         <v>-4.3183220234423196E-3</v>
       </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
@@ -4973,6 +5072,12 @@
         <f t="shared" si="1"/>
         <v>-1.864640883977901E-2</v>
       </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
@@ -5001,8 +5106,14 @@
         <f t="shared" si="1"/>
         <v>-1.112877583465819E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>39511</v>
       </c>
@@ -5029,8 +5140,14 @@
         <f t="shared" si="1"/>
         <v>-4.5454545454545452E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>39539</v>
       </c>
@@ -5057,8 +5174,14 @@
         <f t="shared" si="1"/>
         <v>-1.5374759769378601E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>39574</v>
       </c>
@@ -5085,8 +5208,14 @@
         <f t="shared" si="1"/>
         <v>-2.3060796645702309E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>39602</v>
       </c>
@@ -5113,8 +5242,14 @@
         <f t="shared" si="1"/>
         <v>-1.1371712864250179E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>39630</v>
       </c>
@@ -5141,8 +5276,14 @@
         <f t="shared" si="1"/>
         <v>-3.7414965986394558E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>39665</v>
       </c>
@@ -5169,8 +5310,14 @@
         <f t="shared" si="1"/>
         <v>-4.8192771084337352E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>39693</v>
       </c>
@@ -5197,8 +5344,14 @@
         <f t="shared" si="1"/>
         <v>-2.4492234169653529E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>39728</v>
       </c>
@@ -5225,8 +5378,14 @@
         <f t="shared" si="1"/>
         <v>-5.0267379679144387E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>39756</v>
       </c>
@@ -5253,8 +5412,14 @@
         <f t="shared" si="1"/>
         <v>-3.9027149321266968E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>39784</v>
       </c>
@@ -5281,8 +5446,14 @@
         <f t="shared" si="1"/>
         <v>-2.6875E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>39847</v>
       </c>
@@ -5309,8 +5480,14 @@
         <f t="shared" si="1"/>
         <v>-3.3760186263096632E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>39875</v>
       </c>
@@ -5337,8 +5514,14 @@
         <f t="shared" si="1"/>
         <v>-2.9615626969124131E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>39910</v>
       </c>
@@ -5365,8 +5548,14 @@
         <f t="shared" si="1"/>
         <v>-2.001539645881447E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>39938</v>
       </c>
@@ -5393,8 +5582,14 @@
         <f t="shared" si="1"/>
         <v>-9.5969289827255271E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>39966</v>
       </c>
@@ -5421,8 +5616,14 @@
         <f t="shared" si="1"/>
         <v>-1.2244897959183669E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>40001</v>
       </c>
@@ -5449,6 +5650,12 @@
         <f t="shared" si="1"/>
         <v>1.015228426395939E-2</v>
       </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
@@ -5477,6 +5684,12 @@
         <f t="shared" si="1"/>
         <v>1.163757273482959E-2</v>
       </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
@@ -5505,6 +5718,12 @@
         <f t="shared" si="1"/>
         <v>4.7912388774811769E-3</v>
       </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
@@ -5533,6 +5752,12 @@
         <f t="shared" si="1"/>
         <v>-6.4808813998703816E-3</v>
       </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
@@ -5561,6 +5786,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
@@ -5589,6 +5820,12 @@
         <f t="shared" si="1"/>
         <v>2.167630057803468E-3</v>
       </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
@@ -5617,6 +5854,12 @@
         <f t="shared" si="1"/>
         <v>-6.5217391304347823E-3</v>
       </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
@@ -5645,6 +5888,12 @@
         <f t="shared" si="1"/>
         <v>-1.3764624913971089E-3</v>
       </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
@@ -5673,6 +5922,12 @@
         <f t="shared" si="1"/>
         <v>9.8792535675082324E-3</v>
       </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
@@ -5701,6 +5956,12 @@
         <f t="shared" si="1"/>
         <v>-4.5045045045045036E-3</v>
       </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
@@ -5729,6 +5990,12 @@
         <f t="shared" si="1"/>
         <v>-1.698670605612999E-2</v>
       </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
@@ -5757,6 +6024,12 @@
         <f t="shared" si="1"/>
         <v>-1.2738853503184711E-2</v>
       </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
@@ -5785,6 +6058,12 @@
         <f t="shared" si="1"/>
         <v>-3.7854889589905359E-3</v>
       </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
       <c r="Z44" t="s">
         <v>7</v>
       </c>
@@ -5816,6 +6095,12 @@
         <f t="shared" si="1"/>
         <v>3.9447731755424074E-3</v>
       </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
@@ -5844,6 +6129,12 @@
         <f t="shared" si="1"/>
         <v>-6.8352699931647299E-3</v>
       </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
@@ -5872,6 +6163,12 @@
         <f t="shared" si="1"/>
         <v>-6.1842918985776133E-4</v>
       </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
@@ -5900,8 +6197,14 @@
         <f t="shared" si="1"/>
         <v>4.1493775933609959E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>40575</v>
       </c>
@@ -5928,8 +6231,14 @@
         <f t="shared" si="1"/>
         <v>-6.4184852374839533E-4</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>40603</v>
       </c>
@@ -5956,8 +6265,14 @@
         <f t="shared" si="1"/>
         <v>-5.0983248361252727E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>40638</v>
       </c>
@@ -5984,8 +6299,14 @@
         <f t="shared" si="1"/>
         <v>-3.4572169403630079E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>40666</v>
       </c>
@@ -6012,8 +6333,14 @@
         <f t="shared" si="1"/>
         <v>-1.9973368841544612E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>40701</v>
       </c>
@@ -6040,8 +6367,14 @@
         <f t="shared" si="1"/>
         <v>-1.6178736517719571E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>40729</v>
       </c>
@@ -6068,8 +6401,14 @@
         <f t="shared" si="1"/>
         <v>-1.536098310291859E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>40757</v>
       </c>
@@ -6096,8 +6435,14 @@
         <f t="shared" si="1"/>
         <v>-1.775872627066748E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>40792</v>
       </c>
@@ -6124,8 +6469,14 @@
         <f t="shared" si="1"/>
         <v>-1.918976545842218E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>40820</v>
       </c>
@@ -6152,8 +6503,14 @@
         <f t="shared" si="1"/>
         <v>-1.54320987654321E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>40848</v>
       </c>
@@ -6180,8 +6537,14 @@
         <f t="shared" si="1"/>
         <v>-3.5545023696682458E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>40883</v>
       </c>
@@ -6208,8 +6571,14 @@
         <f t="shared" si="1"/>
         <v>-1.8271257905832752E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>40946</v>
       </c>
@@ -6236,8 +6605,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>40974</v>
       </c>
@@ -6264,8 +6639,14 @@
         <f t="shared" si="1"/>
         <v>-1.6949152542372881E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>41002</v>
       </c>
@@ -6292,8 +6673,14 @@
         <f t="shared" si="1"/>
         <v>-1.60427807486631E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>41030</v>
       </c>
@@ -6320,8 +6707,14 @@
         <f t="shared" si="1"/>
         <v>-2.2079772079772079E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>41065</v>
       </c>
@@ -6348,8 +6741,14 @@
         <f t="shared" si="1"/>
         <v>-3.4965034965034968E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>41093</v>
       </c>
@@ -6376,8 +6775,14 @@
         <f t="shared" si="1"/>
         <v>-1.1874469889737071E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>41128</v>
       </c>
@@ -6404,8 +6809,14 @@
         <f t="shared" si="1"/>
         <v>-2.355858648481091E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>41156</v>
       </c>
@@ -6432,8 +6843,14 @@
         <f t="shared" ref="H67:H130" si="3">G67*-1</f>
         <v>-2.1864951768488749E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>41184</v>
       </c>
@@ -6460,8 +6877,14 @@
         <f t="shared" si="3"/>
         <v>-1.506740681998414E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>41219</v>
       </c>
@@ -6488,8 +6911,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>41247</v>
       </c>
@@ -6516,8 +6945,14 @@
         <f t="shared" si="3"/>
         <v>-1.4672686230248311E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>41310</v>
       </c>
@@ -6544,8 +6979,14 @@
         <f t="shared" si="3"/>
         <v>1.39178844815588E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>41338</v>
       </c>
@@ -6572,8 +7013,14 @@
         <f t="shared" si="3"/>
         <v>1.502629601803156E-3</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>41366</v>
       </c>
@@ -6600,8 +7047,14 @@
         <f t="shared" si="3"/>
         <v>-2.6642984014209588E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>41401</v>
       </c>
@@ -6628,8 +7081,14 @@
         <f t="shared" si="3"/>
         <v>1.407459535538353E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>41429</v>
       </c>
@@ -6656,8 +7115,14 @@
         <f t="shared" si="3"/>
         <v>-1.223491027732463E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>41457</v>
       </c>
@@ -6684,8 +7149,14 @@
         <f t="shared" si="3"/>
         <v>-1.8819503849443971E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>41492</v>
       </c>
@@ -6712,8 +7183,14 @@
         <f t="shared" si="3"/>
         <v>-1.292407108239095E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>41520</v>
       </c>
@@ -6740,8 +7217,14 @@
         <f t="shared" si="3"/>
         <v>-2.1723388848660392E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>41548</v>
       </c>
@@ -6768,8 +7251,14 @@
         <f t="shared" si="3"/>
         <v>8.5959885386819486E-3</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>41583</v>
       </c>
@@ -6796,8 +7285,14 @@
         <f t="shared" si="3"/>
         <v>-9.2236740968485772E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>41611</v>
       </c>
@@ -6824,8 +7319,14 @@
         <f t="shared" si="3"/>
         <v>4.2122999157540014E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>41674</v>
       </c>
@@ -6852,8 +7353,14 @@
         <f t="shared" si="3"/>
         <v>7.2727272727272727E-3</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>41702</v>
       </c>
@@ -6880,8 +7387,14 @@
         <f t="shared" si="3"/>
         <v>-1.295896328293736E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>41730</v>
       </c>
@@ -6908,8 +7421,14 @@
         <f t="shared" si="3"/>
         <v>-5.008347245409015E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>41765</v>
       </c>
@@ -6936,8 +7455,14 @@
         <f t="shared" si="3"/>
         <v>-6.1871616395978348E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>41793</v>
       </c>
@@ -6964,8 +7489,14 @@
         <f t="shared" si="3"/>
         <v>-8.6355785837651123E-3</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>41821</v>
       </c>
@@ -6992,8 +7523,14 @@
         <f t="shared" si="3"/>
         <v>-1.6628873771730911E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>41856</v>
       </c>
@@ -7020,8 +7557,14 @@
         <f t="shared" si="3"/>
         <v>-1.122019635343618E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>41884</v>
       </c>
@@ -7048,8 +7591,14 @@
         <f t="shared" si="3"/>
         <v>-8.6887835703001581E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>41919</v>
       </c>
@@ -7076,8 +7625,14 @@
         <f t="shared" si="3"/>
         <v>-1.461736887360275E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>41947</v>
       </c>
@@ -7104,8 +7659,14 @@
         <f t="shared" si="3"/>
         <v>-1.437371663244353E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>41975</v>
       </c>
@@ -7132,8 +7693,14 @@
         <f t="shared" si="3"/>
         <v>-1.5966386554621851E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>42038</v>
       </c>
@@ -7160,8 +7727,14 @@
         <f t="shared" si="3"/>
         <v>-9.8265895953757228E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>42066</v>
       </c>
@@ -7188,8 +7761,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>42101</v>
       </c>
@@ -7216,8 +7795,14 @@
         <f t="shared" si="3"/>
         <v>-1.396276595744681E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>42129</v>
       </c>
@@ -7244,8 +7829,14 @@
         <f t="shared" si="3"/>
         <v>-1.414514145141451E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>42157</v>
       </c>
@@ -7272,8 +7863,14 @@
         <f t="shared" si="3"/>
         <v>-8.7527352297592995E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>42192</v>
       </c>
@@ -7300,8 +7897,14 @@
         <f t="shared" si="3"/>
         <v>6.1652281134401974E-4</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>42220</v>
       </c>
@@ -7328,8 +7931,14 @@
         <f t="shared" si="3"/>
         <v>6.1199510403916763E-4</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>42248</v>
       </c>
@@ -7356,8 +7965,14 @@
         <f t="shared" si="3"/>
         <v>-1.452145214521452E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I100">
+        <v>1</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>42283</v>
       </c>
@@ -7384,8 +7999,14 @@
         <f t="shared" si="3"/>
         <v>-4.9937578027465668E-3</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>42311</v>
       </c>
@@ -7412,8 +8033,14 @@
         <f t="shared" si="3"/>
         <v>-1.7573696145124721E-2</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>42339</v>
       </c>
@@ -7440,8 +8067,14 @@
         <f t="shared" si="3"/>
         <v>-1.360544217687075E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>42402</v>
       </c>
@@ -7468,8 +8101,14 @@
         <f t="shared" si="3"/>
         <v>-1.6967706622879039E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>42430</v>
       </c>
@@ -7496,8 +8135,14 @@
         <f t="shared" si="3"/>
         <v>-2.777777777777778E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I105">
+        <v>1</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>42465</v>
       </c>
@@ -7524,8 +8169,14 @@
         <f t="shared" si="3"/>
         <v>-6.1659192825112103E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I106">
+        <v>1</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>42493</v>
       </c>
@@ -7552,8 +8203,14 @@
         <f t="shared" si="3"/>
         <v>-8.3582089552238798E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>42528</v>
       </c>
@@ -7580,8 +8237,14 @@
         <f t="shared" si="3"/>
         <v>-1.550868486352357E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I108">
+        <v>1</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>42556</v>
       </c>
@@ -7608,8 +8271,14 @@
         <f t="shared" si="3"/>
         <v>-1.5091863517060371E-2</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I109">
+        <v>1</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>42584</v>
       </c>
@@ -7636,8 +8305,14 @@
         <f t="shared" si="3"/>
         <v>-1.58296943231441E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I110">
+        <v>1</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>42619</v>
       </c>
@@ -7664,8 +8339,14 @@
         <f t="shared" si="3"/>
         <v>-1.175778953556731E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I111">
+        <v>1</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>42647</v>
       </c>
@@ -7692,8 +8373,14 @@
         <f t="shared" si="3"/>
         <v>-3.227541689080151E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>42675</v>
       </c>
@@ -7720,8 +8407,14 @@
         <f t="shared" si="3"/>
         <v>-2.2714366837024418E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>42710</v>
       </c>
@@ -7748,8 +8441,14 @@
         <f t="shared" si="3"/>
         <v>1.3633265167007501E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>42773</v>
       </c>
@@ -7776,8 +8475,14 @@
         <f t="shared" si="3"/>
         <v>1.7720023626698171E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>42801</v>
       </c>
@@ -7804,8 +8509,14 @@
         <f t="shared" si="3"/>
         <v>7.3126142595978062E-3</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>42829</v>
       </c>
@@ -7832,8 +8543,14 @@
         <f t="shared" si="3"/>
         <v>9.8473658296405718E-4</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I117">
+        <v>0</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>42857</v>
       </c>
@@ -7860,8 +8577,14 @@
         <f t="shared" si="3"/>
         <v>5.7925223802001054E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>42892</v>
       </c>
@@ -7888,8 +8611,14 @@
         <f t="shared" si="3"/>
         <v>-6.2642369020501137E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>42920</v>
       </c>
@@ -7916,8 +8645,14 @@
         <f t="shared" si="3"/>
         <v>8.23045267489712E-3</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>42948</v>
       </c>
@@ -7944,8 +8679,14 @@
         <f t="shared" si="3"/>
         <v>5.274261603375527E-4</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>42983</v>
       </c>
@@ -7972,8 +8713,14 @@
         <f t="shared" si="3"/>
         <v>1.4536644457904299E-2</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>43011</v>
       </c>
@@ -8000,8 +8747,14 @@
         <f t="shared" si="3"/>
         <v>-2.5839793281653748E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>43046</v>
       </c>
@@ -8028,8 +8781,14 @@
         <f t="shared" si="3"/>
         <v>1.99700449326011E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>43074</v>
       </c>
@@ -8056,8 +8815,14 @@
         <f t="shared" si="3"/>
         <v>7.926829268292683E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>43137</v>
       </c>
@@ -8084,8 +8849,14 @@
         <f t="shared" si="3"/>
         <v>9.3366093366093368E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I126">
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>43165</v>
       </c>
@@ -8112,8 +8883,14 @@
         <f t="shared" si="3"/>
         <v>4.9109883364027006E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>43193</v>
       </c>
@@ -8140,8 +8917,14 @@
         <f t="shared" si="3"/>
         <v>2.8103044496487119E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I128">
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>43221</v>
       </c>
@@ -8168,8 +8951,14 @@
         <f t="shared" si="3"/>
         <v>6.0150375939849628E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I129">
+        <v>0</v>
+      </c>
+      <c r="J129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>43256</v>
       </c>
@@ -8196,8 +8985,14 @@
         <f t="shared" si="3"/>
         <v>-5.597014925373134E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>43284</v>
       </c>
@@ -8224,8 +9019,14 @@
         <f t="shared" ref="H131:H161" si="5">G131*-1</f>
         <v>4.22654268808115E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>43319</v>
       </c>
@@ -8252,8 +9053,14 @@
         <f t="shared" si="5"/>
         <v>1.4025245441795231E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I132">
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>43347</v>
       </c>
@@ -8280,8 +9087,14 @@
         <f t="shared" si="5"/>
         <v>-5.189413596263622E-4</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>43375</v>
       </c>
@@ -8308,8 +9121,14 @@
         <f t="shared" si="5"/>
         <v>7.855459544383347E-4</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I134">
+        <v>0</v>
+      </c>
+      <c r="J134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>43410</v>
       </c>
@@ -8336,8 +9155,14 @@
         <f t="shared" si="5"/>
         <v>-5.6350238404854792E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I135">
+        <v>0</v>
+      </c>
+      <c r="J135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>43438</v>
       </c>
@@ -8364,8 +9189,14 @@
         <f t="shared" si="5"/>
         <v>-1.2562814070351759E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I136">
+        <v>0</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>43501</v>
       </c>
@@ -8392,8 +9223,14 @@
         <f t="shared" si="5"/>
         <v>-2.4258760107816711E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>43529</v>
       </c>
@@ -8420,8 +9257,14 @@
         <f t="shared" si="5"/>
         <v>-2.6774847870182559E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>43557</v>
       </c>
@@ -8448,8 +9291,14 @@
         <f t="shared" si="5"/>
         <v>-2.506162695152013E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>43592</v>
       </c>
@@ -8476,8 +9325,14 @@
         <f t="shared" si="5"/>
         <v>-1.8207954000958312E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>43620</v>
       </c>
@@ -8504,8 +9359,14 @@
         <f t="shared" si="5"/>
         <v>-1.407129455909944E-2</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>43648</v>
       </c>
@@ -8532,8 +9393,14 @@
         <f t="shared" si="5"/>
         <v>-1.016456921587609E-2</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I142">
+        <v>0</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>43683</v>
       </c>
@@ -8560,8 +9427,14 @@
         <f t="shared" si="5"/>
         <v>-9.2592592592592587E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>43711</v>
       </c>
@@ -8588,8 +9461,14 @@
         <f t="shared" si="5"/>
         <v>-2.7353689567430031E-2</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I144">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>43739</v>
       </c>
@@ -8616,8 +9495,14 @@
         <f t="shared" si="5"/>
         <v>-1.7063313875168389E-2</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>43774</v>
       </c>
@@ -8644,8 +9529,14 @@
         <f t="shared" si="5"/>
         <v>-1.441190144119014E-2</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>43802</v>
       </c>
@@ -8672,8 +9563,14 @@
         <f t="shared" si="5"/>
         <v>-1.814882032667877E-2</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I147">
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>43865</v>
       </c>
@@ -8700,8 +9597,14 @@
         <f t="shared" si="5"/>
         <v>-1.7738359201773839E-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I148">
+        <v>0</v>
+      </c>
+      <c r="J148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>43893</v>
       </c>
@@ -8728,8 +9631,14 @@
         <f t="shared" si="5"/>
         <v>-3.3149171270718231E-2</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>43908</v>
       </c>
@@ -8756,8 +9665,14 @@
         <f t="shared" si="5"/>
         <v>-8.7660148347943351E-3</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I150">
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>43928</v>
       </c>
@@ -8784,8 +9699,14 @@
         <f t="shared" si="5"/>
         <v>-2.265659706796979E-2</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>43956</v>
       </c>
@@ -8812,8 +9733,14 @@
         <f t="shared" si="5"/>
         <v>-3.3216100039077767E-2</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>43984</v>
       </c>
@@ -8840,8 +9767,14 @@
         <f t="shared" si="5"/>
         <v>-3.5638297872340428E-2</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>44019</v>
       </c>
@@ -8868,8 +9801,14 @@
         <f t="shared" si="5"/>
         <v>-3.411633109619687E-2</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" s="3">
         <v>44047</v>
       </c>
@@ -8896,8 +9835,14 @@
         <f t="shared" si="5"/>
         <v>-2.5747508305647839E-2</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>44075</v>
       </c>
@@ -8924,8 +9869,14 @@
         <f t="shared" si="5"/>
         <v>-1.6868740115972589E-2</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" s="3">
         <v>44110</v>
       </c>
@@ -8952,8 +9903,14 @@
         <f t="shared" si="5"/>
         <v>-4.589261128958238E-3</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" s="3">
         <v>44138</v>
       </c>
@@ -8980,8 +9937,14 @@
         <f t="shared" si="5"/>
         <v>1.1301989150090419E-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" s="3">
         <v>44166</v>
       </c>
@@ -9008,8 +9971,14 @@
         <f t="shared" si="5"/>
         <v>-2.8392958546280518E-3</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" s="3">
         <v>44229</v>
       </c>
@@ -9036,8 +10005,14 @@
         <f t="shared" si="5"/>
         <v>1.9230769230769228E-2</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" s="3">
         <v>44257</v>
       </c>
@@ -9064,10 +10039,17 @@
         <f t="shared" si="5"/>
         <v>6.5975494816211122E-3</v>
       </c>
+      <c r="I161">
+        <v>0</v>
+      </c>
+      <c r="J161">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>